<commit_message>
Add OneSignal debug endpoints and better logging
</commit_message>
<xml_diff>
--- a/VAKA FORMU.csv.xlsx
+++ b/VAKA FORMU.csv.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\HEALMEDY\ABROV2\lockdownsofthbys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{396C676D-C0EF-4482-B276-2FAEB5F19C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3C19D219-9603-4308-89A0-73728D2D3CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VAKA FORMU" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 

</xml_diff>